<commit_message>
Update combined met (MetaboDiff) and prot pathway analysis results.xlsx
</commit_message>
<xml_diff>
--- a/Pathway analysis/4th pathway analysis using MetaboDiff results/combined met (MetaboDiff) and prot pathway analysis results.xlsx
+++ b/Pathway analysis/4th pathway analysis using MetaboDiff results/combined met (MetaboDiff) and prot pathway analysis results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/Pathway analysis/4th pathway analysis using MetaboDiff results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8EB90243-8658-4877-B959-A7D16221D041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{8EB90243-8658-4877-B959-A7D16221D041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{73D3D39E-427F-4370-AC5D-546480316DD3}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="0" windowWidth="9730" windowHeight="9740"/>
+    <workbookView xWindow="9250" yWindow="0" windowWidth="9890" windowHeight="10150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined met (MetaboDiff) and p" sheetId="1" r:id="rId1"/>
@@ -1819,7 +1819,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2663,7 +2663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H590"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2672,7 +2672,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="100.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>

</xml_diff>